<commit_message>
report - from david, ignore highlights/comments, not where where a clean one is.
</commit_message>
<xml_diff>
--- a/BackendData/UIGeneralInfo.xlsx
+++ b/BackendData/UIGeneralInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmcgrath\Documents\GitHub\CanCurve\RevisedSample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmcgrath\Documents\GitHub\CanCurve\BackendData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399343DD-8A6F-4085-B21E-743694510DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A702F8B7-6F4E-4A71-9BA6-F69928EE878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{6CA9E30C-38E9-4BE8-8C33-31C3FBABF0B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{6CA9E30C-38E9-4BE8-8C33-31C3FBABF0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralInfo" sheetId="3" r:id="rId1"/>
@@ -1199,10 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859A1630-8B15-4C82-9C11-258080034893}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,10 +2104,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96924F24-1B2C-43E1-83B2-25B6BBEBBA2E}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>